<commit_message>
fixed code best third teams
right sorting order for goals happening the last day
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/uefa/wc/best_four_third_teams_wc_eufa.xlsx
+++ b/data/out/wiki/men/uefa/wc/best_four_third_teams_wc_eufa.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -594,7 +594,7 @@
         <v>1986</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -668,7 +668,7 @@
         <v>1986</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -742,47 +742,47 @@
         <v>1986</v>
       </c>
       <c r="B5" t="n">
+        <v>62</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1986-06-09</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Group C</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>['Belgium', 'Italy', 'Morocco', 'Northern Ireland']</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>['Uruguay', 'Hungary']</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1986-06-09</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Group C</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>['Belgium', 'Bulgaria', 'Northern Ireland', 'Poland']</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>['Uruguay', 'Hungary']</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>['Bulgaria', 'Northern Ireland']</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>1</v>
       </c>
-      <c r="J5" t="n">
-        <v>2</v>
-      </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>['Bulgaria', 2, -1, 2]</t>
+          <t>['Italy', 3, 0, 2]</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -807,7 +807,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -816,7 +816,7 @@
         <v>1986</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -835,7 +835,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['Belgium', 'Bulgaria', 'Northern Ireland', 'Poland']</t>
+          <t>['Belgium', 'Italy', 'Morocco', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -845,18 +845,18 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Northern Ireland']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>['Bulgaria', 2, -1, 2]</t>
+          <t>['Italy', 3, 0, 2]</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -881,7 +881,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -890,7 +890,7 @@
         <v>1986</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -909,7 +909,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>['Belgium', 'Bulgaria', 'Northern Ireland', 'Poland']</t>
+          <t>['Belgium', 'Italy', 'Morocco', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -919,18 +919,18 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Northern Ireland']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>['Bulgaria', 2, -1, 2]</t>
+          <t>['Italy', 3, 0, 2]</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -955,7 +955,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -964,11 +964,11 @@
         <v>1986</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-10</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -978,12 +978,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group A</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>['Belgium', 'Bulgaria', 'Northern Ireland', 'Poland']</t>
+          <t>['Belgium', 'Bulgaria', 'Morocco', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
         <v>2</v>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -1038,11 +1038,11 @@
         <v>1986</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-10</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1052,12 +1052,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group A</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>['Belgium', 'Bulgaria', 'Northern Ireland', 'Poland']</t>
+          <t>['Belgium', 'Bulgaria', 'Morocco', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -1112,11 +1112,11 @@
         <v>1986</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-10</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1126,12 +1126,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group A</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>['Belgium', 'Bulgaria', 'Northern Ireland', 'Poland']</t>
+          <t>['Belgium', 'Bulgaria', 'Morocco', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -1186,11 +1186,11 @@
         <v>1986</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-10</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1200,12 +1200,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group A</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>['Belgium', 'Bulgaria', 'Northern Ireland', 'Poland']</t>
+          <t>['Belgium', 'Bulgaria', 'Morocco', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1251,7 +1251,7 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -1260,11 +1260,11 @@
         <v>1986</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-10</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1274,12 +1274,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group A</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>['Belgium', 'Bulgaria', 'Northern Ireland', 'Poland']</t>
+          <t>['Belgium', 'Bulgaria', 'Morocco', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -1334,11 +1334,11 @@
         <v>1986</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-10</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1348,12 +1348,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group A</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>['Belgium', 'Bulgaria', 'Northern Ireland', 'Poland']</t>
+          <t>['Belgium', 'Bulgaria', 'Morocco', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -1408,11 +1408,11 @@
         <v>1986</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-11</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1422,12 +1422,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Northern Ireland', 'Paraguay', 'Poland']</t>
+          <t>['Bulgaria', 'Morocco', 'Northern Ireland', 'Paraguay']</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -1482,11 +1482,11 @@
         <v>1986</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-11</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1496,12 +1496,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>['Belgium', 'Bulgaria', 'Northern Ireland', 'Poland']</t>
+          <t>['Belgium', 'Bulgaria', 'Morocco', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -1556,11 +1556,11 @@
         <v>1986</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-11</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1570,12 +1570,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>['Belgium', 'Bulgaria', 'Northern Ireland', 'Poland']</t>
+          <t>['Belgium', 'Bulgaria', 'Morocco', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -1630,11 +1630,11 @@
         <v>1986</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-11</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1644,12 +1644,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Northern Ireland', 'Paraguay', 'Poland']</t>
+          <t>['Bulgaria', 'Morocco', 'Northern Ireland', 'Paraguay']</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1695,7 +1695,7 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -1704,11 +1704,11 @@
         <v>1986</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-11</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1718,12 +1718,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>['Belgium', 'Bulgaria', 'Northern Ireland', 'Poland']</t>
+          <t>['Belgium', 'Bulgaria', 'Morocco', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>['Poland', 3, -2, 1]</t>
+          <t>['Morocco', 3, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -1778,21 +1778,21 @@
         <v>1986</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-11</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group F</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1852,21 +1852,21 @@
         <v>1986</v>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-11</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group F</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1926,21 +1926,21 @@
         <v>1986</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-11</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group F</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2000,21 +2000,21 @@
         <v>1986</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-11</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group F</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2074,21 +2074,21 @@
         <v>1986</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-11</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group F</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2148,21 +2148,21 @@
         <v>1986</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-11</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group F</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2222,11 +2222,11 @@
         <v>1986</v>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-12</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group D</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2296,11 +2296,11 @@
         <v>1986</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-12</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2310,7 +2310,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group D</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2370,11 +2370,11 @@
         <v>1986</v>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-12</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2384,7 +2384,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group D</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2444,11 +2444,11 @@
         <v>1986</v>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-12</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2458,7 +2458,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group D</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2518,11 +2518,11 @@
         <v>1986</v>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-12</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2532,7 +2532,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group D</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2592,11 +2592,11 @@
         <v>1986</v>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1986-06-09</t>
+          <t>1986-06-13</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Group C</t>
+          <t>Group E</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2666,13 +2666,21 @@
         <v>1990</v>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
-      </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>1990-06-18</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2687,7 +2695,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>['Argentina', 'Colombia']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2703,7 +2711,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>['Argentina', 2, 1, 2]</t>
+          <t>['Argentina', 3, 1, 2]</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
@@ -2732,13 +2740,21 @@
         <v>1990</v>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
-      </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
+        <v>29</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>1990-06-18</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2798,13 +2814,21 @@
         <v>1990</v>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
-      </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
+        <v>52</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>1990-06-18</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2850,7 +2874,7 @@
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2864,18 +2888,26 @@
         <v>1990</v>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
-      </c>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
+        <v>62</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1990-06-18</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>['Argentina', 'Colombia', 'Ireland', 'Scotland']</t>
+          <t>['Colombia', 'Ireland', 'Romania', 'Scotland']</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -2889,10 +2921,10 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
@@ -2901,7 +2933,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>['Argentina', 3, 1, 2]</t>
+          <t>['Romania', 2, 0, 3]</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
@@ -2916,7 +2948,7 @@
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -2930,32 +2962,40 @@
         <v>1990</v>
       </c>
       <c r="B35" t="n">
+        <v>63</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>1990-06-18</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Group B</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>['Colombia', 'Ireland', 'Romania', 'Scotland']</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>['Uruguay', 'Austria']</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
         <v>0</v>
-      </c>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Group A</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>['Colombia', 'Ireland', 'Romania', 'Scotland']</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>['Uruguay', 'Austria']</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="I35" t="n">
-        <v>1</v>
       </c>
       <c r="J35" t="n">
         <v>1</v>
@@ -2982,7 +3022,7 @@
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -2996,28 +3036,36 @@
         <v>1990</v>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
+        <v>68</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>1990-06-18</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>['Austria', 'Colombia', 'Romania', 'Scotland']</t>
+          <t>['Argentina', 'Colombia', 'Ireland', 'Scotland']</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>['Ireland', 'Uruguay']</t>
+          <t>['Uruguay', 'Austria']</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>['Austria', 'Scotland']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3028,12 +3076,12 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>['Austria', 2, 0, 2]</t>
+          <t>['Austria', 0, -2, 0]</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>['Romania', 2, 0, 3]</t>
+          <t>['Argentina', 3, 1, 3]</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
@@ -3048,7 +3096,7 @@
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3062,39 +3110,47 @@
         <v>1990</v>
       </c>
       <c r="B37" t="n">
+        <v>5</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>1990-06-19</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Group D</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>['Argentina', 'Colombia', 'Ireland', 'Scotland']</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>['Uruguay', 'Austria']</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
         <v>0</v>
       </c>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Group A</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>['Argentina', 'Austria', 'Colombia', 'Scotland']</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>['Ireland', 'Uruguay']</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>['Austria', 'Scotland']</t>
-        </is>
-      </c>
-      <c r="I37" t="n">
-        <v>1</v>
-      </c>
       <c r="J37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>['Austria', 2, 0, 2]</t>
+          <t>['Austria', 0, -2, 0]</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3109,12 +3165,12 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>['Colombia', 2, 1, 2]</t>
+          <t>['Colombia', 3, 1, 2]</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3128,39 +3184,47 @@
         <v>1990</v>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
-      </c>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
+        <v>9</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>1990-06-19</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group D</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>['Argentina', 'Austria', 'Colombia', 'Scotland']</t>
+          <t>['Argentina', 'Colombia', 'Ireland', 'Scotland']</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>['Ireland', 'Uruguay']</t>
+          <t>['Uruguay', 'Austria']</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>['Austria', 'Scotland']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I38" t="n">
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>['Austria', 2, 0, 2]</t>
+          <t>['Austria', 0, -2, 0]</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3180,7 +3244,7 @@
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3194,39 +3258,47 @@
         <v>1990</v>
       </c>
       <c r="B39" t="n">
+        <v>22</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>1990-06-19</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Group D</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>['Argentina', 'Colombia', 'Ireland', 'Scotland']</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>['Uruguay', 'Austria']</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
         <v>0</v>
       </c>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>Group A</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>['Argentina', 'Colombia', 'Ireland', 'Scotland']</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>['Uruguay', 'Austria']</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="I39" t="n">
-        <v>1</v>
-      </c>
       <c r="J39" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>['Austria', 1, -2, 0]</t>
+          <t>['Austria', 0, -2, 0]</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3246,7 +3318,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3260,13 +3332,21 @@
         <v>1990</v>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
-      </c>
-      <c r="C40" t="inlineStr"/>
-      <c r="D40" t="inlineStr"/>
+        <v>46</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>1990-06-19</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group D</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3288,11 +3368,11 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>['Austria', 1, -2, 0]</t>
+          <t>['Austria', 0, -2, 0]</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3312,7 +3392,7 @@
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3326,13 +3406,21 @@
         <v>1990</v>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
-      </c>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
+        <v>88</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>1990-06-19</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group D</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3347,18 +3435,18 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Scotland', 'Colombia']</t>
         </is>
       </c>
       <c r="I41" t="n">
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>['Austria', 1, -2, 0]</t>
+          <t>['Austria', 0, -2, 0]</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3373,12 +3461,12 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>['Colombia', 3, 1, 2]</t>
+          <t>['Colombia', 2, 0, 2]</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3392,13 +3480,21 @@
         <v>1990</v>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
-      </c>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
+        <v>93</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>1990-06-19</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group D</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3413,18 +3509,18 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>['Scotland', 'Colombia']</t>
+          <t>['Argentina', 'Colombia']</t>
         </is>
       </c>
       <c r="I42" t="n">
         <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>['Austria', 1, -2, 0]</t>
+          <t>['Austria', 0, -2, 0]</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3439,12 +3535,12 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>['Colombia', 2, 0, 2]</t>
+          <t>['Colombia', 3, 1, 3]</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3458,10 +3554,18 @@
         <v>1990</v>
       </c>
       <c r="B43" t="n">
-        <v>0</v>
-      </c>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
+        <v>49</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>1990-06-19</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E43" t="inlineStr">
         <is>
           <t>Group A</t>
@@ -3474,7 +3578,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>['Uruguay', 'Austria']</t>
+          <t>['Austria', 'Uruguay']</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -3486,11 +3590,11 @@
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>['Austria', 1, -2, 0]</t>
+          <t>['Austria', 2, -1, 1]</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3510,7 +3614,7 @@
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3524,10 +3628,18 @@
         <v>1990</v>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
-      </c>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
+        <v>78</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>1990-06-19</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E44" t="inlineStr">
         <is>
           <t>Group A</t>
@@ -3535,28 +3647,28 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>['Argentina', 'Colombia', 'Ireland', 'Scotland']</t>
+          <t>['Argentina', 'Austria', 'Colombia', 'Scotland']</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>['Austria', 'Uruguay']</t>
+          <t>['Ireland', 'Uruguay']</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>['Argentina', 'Colombia']</t>
+          <t>['Austria', 'Argentina', 'Scotland', 'Colombia']</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>['Austria', 2, -1, 1]</t>
+          <t>['Austria', 2, 0, 2]</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3576,7 +3688,7 @@
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3590,10 +3702,18 @@
         <v>1990</v>
       </c>
       <c r="B45" t="n">
-        <v>0</v>
-      </c>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
+        <v>83</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>1990-06-19</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E45" t="inlineStr">
         <is>
           <t>Group A</t>
@@ -3601,28 +3721,28 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>['Argentina', 'Austria', 'Colombia', 'Scotland']</t>
+          <t>['Argentina', 'Colombia', 'Ireland', 'Scotland']</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>['Ireland', 'Uruguay']</t>
+          <t>['Austria', 'Uruguay']</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>['Austria', 'Argentina', 'Scotland', 'Colombia']</t>
+          <t>['Argentina', 'Colombia']</t>
         </is>
       </c>
       <c r="I45" t="n">
         <v>1</v>
       </c>
       <c r="J45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>['Austria', 2, 0, 2]</t>
+          <t>['Austria', 2, -1, 2]</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3642,7 +3762,7 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3656,18 +3776,26 @@
         <v>1990</v>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
-      </c>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
+        <v>32</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>1990-06-20</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group C</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>['Argentina', 'Colombia', 'Ireland', 'Scotland']</t>
+          <t>['Argentina', 'Colombia', 'Ireland', 'Sweden']</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -3684,7 +3812,7 @@
         <v>1</v>
       </c>
       <c r="J46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
@@ -3698,7 +3826,7 @@
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>['Scotland', 2, 0, 2]</t>
+          <t>['Sweden', 2, -1, 3]</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
@@ -3708,7 +3836,7 @@
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3722,18 +3850,26 @@
         <v>1990</v>
       </c>
       <c r="B47" t="n">
-        <v>0</v>
-      </c>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
+        <v>75</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>1990-06-20</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group C</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>['Argentina', 'Colombia', 'Ireland', 'Sweden']</t>
+          <t>['Argentina', 'Colombia', 'Ireland', 'Scotland']</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -3750,7 +3886,7 @@
         <v>1</v>
       </c>
       <c r="J47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -3764,7 +3900,7 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>['Sweden', 2, -1, 3]</t>
+          <t>['Scotland', 3, 0, 2]</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
@@ -3774,7 +3910,7 @@
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3788,35 +3924,43 @@
         <v>1990</v>
       </c>
       <c r="B48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
+        <v>81</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>1990-06-20</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group C</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>['Argentina', 'Colombia', 'Ireland', 'Scotland']</t>
+          <t>['Argentina', 'Austria', 'Colombia', 'Ireland']</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>['Austria', 'Uruguay']</t>
+          <t>['Scotland', 'Uruguay']</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>['Argentina', 'Colombia']</t>
+          <t>['Austria', 'Argentina', 'Scotland', 'Colombia']</t>
         </is>
       </c>
       <c r="I48" t="n">
         <v>1</v>
       </c>
       <c r="J48" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K48" t="inlineStr">
         <is>
@@ -3830,7 +3974,7 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>['Scotland', 3, 0, 2]</t>
+          <t>['Scotland', 2, -1, 2]</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
@@ -3840,7 +3984,7 @@
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -3854,35 +3998,43 @@
         <v>1990</v>
       </c>
       <c r="B49" t="n">
+        <v>87</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>1990-06-20</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Group C</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>['Argentina', 'Austria', 'Colombia', 'Ireland']</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>['Scotland', 'Uruguay']</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>['Austria', 'Argentina', 'Scotland', 'Colombia']</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
         <v>0</v>
       </c>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>Group A</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>['Argentina', 'Austria', 'Colombia', 'Ireland']</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>['Scotland', 'Uruguay']</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>['Austria', 'Argentina', 'Scotland', 'Colombia']</t>
-        </is>
-      </c>
-      <c r="I49" t="n">
-        <v>1</v>
-      </c>
       <c r="J49" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
@@ -3906,7 +4058,7 @@
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -3920,13 +4072,21 @@
         <v>1990</v>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
-      </c>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
+        <v>26</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>1990-06-21</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group E</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -3948,7 +4108,7 @@
         <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
@@ -3986,13 +4146,21 @@
         <v>1990</v>
       </c>
       <c r="B51" t="n">
-        <v>0</v>
-      </c>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
+        <v>38</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>1990-06-21</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group E</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4014,7 +4182,7 @@
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -4052,23 +4220,31 @@
         <v>1990</v>
       </c>
       <c r="B52" t="n">
-        <v>0</v>
-      </c>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
+        <v>91</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>1990-06-21</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group E</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>['Argentina', 'Austria', 'Colombia', 'Ireland']</t>
+          <t>['Argentina', 'Colombia', 'Ireland', 'Uruguay']</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>['Scotland', 'Uruguay']</t>
+          <t>['Austria', 'Scotland']</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -4077,10 +4253,10 @@
         </is>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
@@ -4104,7 +4280,7 @@
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>['Uruguay', 2, -2, 1]</t>
+          <t>['Uruguay', 3, -1, 2]</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4118,18 +4294,26 @@
         <v>1990</v>
       </c>
       <c r="B53" t="n">
-        <v>0</v>
-      </c>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
+        <v>11</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>1990-06-21</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group F</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>['Argentina', 'Colombia', 'Ireland', 'Uruguay']</t>
+          <t>['Argentina', 'Colombia', 'Egypt', 'Uruguay']</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -4146,7 +4330,7 @@
         <v>1</v>
       </c>
       <c r="J53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K53" t="inlineStr">
         <is>
@@ -4175,7 +4359,7 @@
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>['Ireland', 2, 0, 1]</t>
+          <t>['Egypt', 3, 0, 1]</t>
         </is>
       </c>
     </row>
@@ -4184,23 +4368,31 @@
         <v>1990</v>
       </c>
       <c r="B54" t="n">
-        <v>0</v>
-      </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
+        <v>58</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>1990-06-21</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group F</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>['Argentina', 'Colombia', 'Egypt', 'Uruguay']</t>
+          <t>['Argentina', 'Austria', 'Colombia', 'Uruguay']</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>['Austria', 'Scotland']</t>
+          <t>['Scotland', 'Egypt']</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -4212,7 +4404,7 @@
         <v>1</v>
       </c>
       <c r="J54" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K54" t="inlineStr">
         <is>
@@ -4241,7 +4433,7 @@
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>['Egypt', 3, 0, 1]</t>
+          <t>['Egypt', 2, -1, 1]</t>
         </is>
       </c>
     </row>
@@ -4250,23 +4442,31 @@
         <v>1990</v>
       </c>
       <c r="B55" t="n">
-        <v>0</v>
-      </c>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
+        <v>71</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>1990-06-21</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group F</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>['Argentina', 'Austria', 'Colombia', 'Uruguay']</t>
+          <t>['Argentina', 'Colombia', 'Ireland', 'Uruguay']</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>['Scotland', 'Egypt']</t>
+          <t>['Austria', 'Scotland']</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -4278,7 +4478,7 @@
         <v>1</v>
       </c>
       <c r="J55" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K55" t="inlineStr">
         <is>
@@ -4307,7 +4507,7 @@
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>['Egypt', 2, -1, 1]</t>
+          <t>['Ireland', 3, 0, 2]</t>
         </is>
       </c>
     </row>
@@ -4327,53 +4527,53 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>['Argentina', 'Colombia', 'Ireland', 'Uruguay']</t>
+          <t>['Argentina', 'Colombia', 'Ireland', 'Scotland']</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>['Austria', 'Scotland']</t>
+          <t>['Uruguay', 'Austria']</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>['Austria', 'Argentina', 'Scotland', 'Colombia']</t>
+          <t>['Argentina', 'Colombia']</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>['Austria', 2, -1, 2]</t>
+          <t>['Austria', 0, -2, 0]</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>['Argentina', 3, 1, 3]</t>
+          <t>['Argentina', 2, 1, 2]</t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>['Scotland', 2, -1, 2]</t>
+          <t>['Scotland', 2, 0, 2]</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>['Colombia', 3, 1, 3]</t>
+          <t>['Colombia', 2, 1, 2]</t>
         </is>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>['Uruguay', 3, -1, 2]</t>
+          <t>['Uruguay', 1, -2, 1]</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>['Ireland', 3, 0, 2]</t>
+          <t>['Ireland', 2, 0, 1]</t>
         </is>
       </c>
     </row>
@@ -4456,7 +4656,7 @@
         <v>1994</v>
       </c>
       <c r="B58" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -4530,7 +4730,7 @@
         <v>1994</v>
       </c>
       <c r="B59" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -4554,7 +4754,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>['Russia', 'South Korea']</t>
+          <t>['South Korea', 'Cameroon']</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -4575,7 +4775,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>['Russia', 3, -1, 4]</t>
+          <t>['Cameroon', 1, -3, 2]</t>
         </is>
       </c>
       <c r="M59" t="inlineStr">
@@ -4604,7 +4804,7 @@
         <v>1994</v>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -4628,7 +4828,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>['Russia', 'South Korea']</t>
+          <t>['South Korea', 'Cameroon']</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -4649,7 +4849,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>['Russia', 3, -1, 4]</t>
+          <t>['Cameroon', 1, -3, 2]</t>
         </is>
       </c>
       <c r="M60" t="inlineStr">
@@ -4678,11 +4878,11 @@
         <v>1994</v>
       </c>
       <c r="B61" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-27</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -4692,7 +4892,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group C</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -4702,7 +4902,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>['Russia', 'South Korea']</t>
+          <t>['South Korea', 'Cameroon']</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -4723,7 +4923,7 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>['Russia', 3, -1, 4]</t>
+          <t>['Cameroon', 1, -3, 2]</t>
         </is>
       </c>
       <c r="M61" t="inlineStr">
@@ -4752,11 +4952,11 @@
         <v>1994</v>
       </c>
       <c r="B62" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-27</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -4766,7 +4966,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group C</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -4776,7 +4976,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>['Russia', 'South Korea']</t>
+          <t>['South Korea', 'Cameroon']</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -4797,7 +4997,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>['Russia', 3, -1, 4]</t>
+          <t>['Cameroon', 1, -3, 2]</t>
         </is>
       </c>
       <c r="M62" t="inlineStr">
@@ -4826,11 +5026,11 @@
         <v>1994</v>
       </c>
       <c r="B63" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-27</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -4840,7 +5040,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group C</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -4850,7 +5050,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>['Russia', 'South Korea']</t>
+          <t>['South Korea', 'Cameroon']</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -4871,7 +5071,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>['Russia', 3, -1, 4]</t>
+          <t>['Cameroon', 1, -3, 2]</t>
         </is>
       </c>
       <c r="M63" t="inlineStr">
@@ -4900,11 +5100,11 @@
         <v>1994</v>
       </c>
       <c r="B64" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-27</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -4914,7 +5114,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group C</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -4924,7 +5124,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>['Russia', 'South Korea']</t>
+          <t>['South Korea', 'Cameroon']</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -4945,7 +5145,7 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>['Russia', 3, -1, 4]</t>
+          <t>['Cameroon', 1, -3, 2]</t>
         </is>
       </c>
       <c r="M64" t="inlineStr">
@@ -4974,11 +5174,11 @@
         <v>1994</v>
       </c>
       <c r="B65" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-27</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -4988,7 +5188,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group C</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -4998,7 +5198,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>['Russia', 'South Korea']</t>
+          <t>['South Korea', 'Cameroon']</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -5019,7 +5219,7 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>['Russia', 3, -1, 4]</t>
+          <t>['Cameroon', 1, -3, 2]</t>
         </is>
       </c>
       <c r="M65" t="inlineStr">
@@ -5048,11 +5248,11 @@
         <v>1994</v>
       </c>
       <c r="B66" t="n">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-27</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -5062,7 +5262,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group C</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5072,7 +5272,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>['Russia', 'South Korea']</t>
+          <t>['South Korea', 'Cameroon']</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -5093,7 +5293,7 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>['Russia', 3, -1, 4]</t>
+          <t>['Cameroon', 1, -3, 2]</t>
         </is>
       </c>
       <c r="M66" t="inlineStr">
@@ -5122,11 +5322,11 @@
         <v>1994</v>
       </c>
       <c r="B67" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-27</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5136,7 +5336,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group C</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5146,7 +5346,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>['Russia', 'South Korea']</t>
+          <t>['South Korea', 'Cameroon']</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -5167,7 +5367,7 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>['Russia', 3, -1, 4]</t>
+          <t>['Cameroon', 1, -3, 2]</t>
         </is>
       </c>
       <c r="M67" t="inlineStr">
@@ -5196,11 +5396,11 @@
         <v>1994</v>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-27</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5210,7 +5410,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group C</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5220,7 +5420,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>['Russia', 'South Korea']</t>
+          <t>['South Korea', 'Cameroon']</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -5241,7 +5441,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>['Russia', 3, -1, 4]</t>
+          <t>['Cameroon', 1, -3, 2]</t>
         </is>
       </c>
       <c r="M68" t="inlineStr">
@@ -5270,11 +5470,11 @@
         <v>1994</v>
       </c>
       <c r="B69" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-27</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5284,7 +5484,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group C</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5294,7 +5494,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>['Russia', 'South Korea']</t>
+          <t>['South Korea', 'Cameroon']</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -5315,7 +5515,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>['Russia', 3, -1, 4]</t>
+          <t>['Cameroon', 1, -3, 2]</t>
         </is>
       </c>
       <c r="M69" t="inlineStr">
@@ -5344,21 +5544,21 @@
         <v>1994</v>
       </c>
       <c r="B70" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-28</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group E</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5368,7 +5568,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>['Russia', 'South Korea']</t>
+          <t>['South Korea', 'Cameroon']</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -5389,7 +5589,7 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>['Russia', 3, -1, 4]</t>
+          <t>['Cameroon', 1, -3, 2]</t>
         </is>
       </c>
       <c r="M70" t="inlineStr">
@@ -5418,21 +5618,21 @@
         <v>1994</v>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-28</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group E</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5442,7 +5642,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>['Russia', 'South Korea']</t>
+          <t>['South Korea', 'Cameroon']</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -5463,7 +5663,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>['Russia', 3, -1, 4]</t>
+          <t>['Cameroon', 1, -3, 2]</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
@@ -5492,11 +5692,11 @@
         <v>1994</v>
       </c>
       <c r="B72" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-28</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -5506,7 +5706,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5566,11 +5766,11 @@
         <v>1994</v>
       </c>
       <c r="B73" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-28</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -5580,7 +5780,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5640,11 +5840,11 @@
         <v>1994</v>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-28</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -5654,7 +5854,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5714,11 +5914,11 @@
         <v>1994</v>
       </c>
       <c r="B75" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-28</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -5728,7 +5928,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -5788,43 +5988,43 @@
         <v>1994</v>
       </c>
       <c r="B76" t="n">
+        <v>47</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>1994-06-28</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Group B</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>['Bulgaria', 'Italy', 'Saudi Arabia', 'United States']</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>['Russia', 'South Korea']</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>['United States', 'Saudi Arabia']</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
         <v>0</v>
       </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>1994-06-26</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>20:00</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>Group A</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>['Bulgaria', 'Italy', 'Netherlands', 'United States']</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>['Russia', 'South Korea']</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>['United States', 'Netherlands']</t>
-        </is>
-      </c>
-      <c r="I76" t="n">
-        <v>1</v>
-      </c>
       <c r="J76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K76" t="inlineStr">
         <is>
@@ -5853,7 +6053,7 @@
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>['Netherlands', 4, 0, 3]</t>
+          <t>['Saudi Arabia', 4, 0, 3]</t>
         </is>
       </c>
     </row>
@@ -5862,11 +6062,11 @@
         <v>1994</v>
       </c>
       <c r="B77" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-28</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -5876,12 +6076,12 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Italy', 'Netherlands', 'United States']</t>
+          <t>['Bulgaria', 'Italy', 'Saudi Arabia', 'United States']</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -5891,14 +6091,14 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>['United States', 'Netherlands']</t>
+          <t>['United States', 'Saudi Arabia']</t>
         </is>
       </c>
       <c r="I77" t="n">
         <v>0</v>
       </c>
       <c r="J77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K77" t="inlineStr">
         <is>
@@ -5927,7 +6127,7 @@
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>['Netherlands', 4, 0, 3]</t>
+          <t>['Saudi Arabia', 4, 0, 3]</t>
         </is>
       </c>
     </row>
@@ -5936,11 +6136,11 @@
         <v>1994</v>
       </c>
       <c r="B78" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-28</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -5950,12 +6150,12 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Italy', 'Netherlands', 'United States']</t>
+          <t>['Bulgaria', 'Italy', 'Saudi Arabia', 'United States']</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -5965,14 +6165,14 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>['United States', 'Netherlands']</t>
+          <t>['United States', 'Saudi Arabia']</t>
         </is>
       </c>
       <c r="I78" t="n">
         <v>0</v>
       </c>
       <c r="J78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K78" t="inlineStr">
         <is>
@@ -6001,7 +6201,7 @@
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>['Netherlands', 4, 0, 3]</t>
+          <t>['Saudi Arabia', 4, 0, 3]</t>
         </is>
       </c>
     </row>
@@ -6010,11 +6210,11 @@
         <v>1994</v>
       </c>
       <c r="B79" t="n">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-28</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -6024,12 +6224,12 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group B</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Italy', 'Netherlands', 'United States']</t>
+          <t>['Bulgaria', 'Italy', 'Saudi Arabia', 'United States']</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -6039,14 +6239,14 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>['United States', 'Netherlands']</t>
+          <t>['United States', 'Saudi Arabia']</t>
         </is>
       </c>
       <c r="I79" t="n">
         <v>0</v>
       </c>
       <c r="J79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K79" t="inlineStr">
         <is>
@@ -6075,7 +6275,7 @@
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>['Netherlands', 4, 0, 3]</t>
+          <t>['Saudi Arabia', 4, 0, 3]</t>
         </is>
       </c>
     </row>
@@ -6084,21 +6284,21 @@
         <v>1994</v>
       </c>
       <c r="B80" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-29</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group F</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6117,7 +6317,7 @@
         </is>
       </c>
       <c r="I80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J80" t="n">
         <v>4</v>
@@ -6158,21 +6358,21 @@
         <v>1994</v>
       </c>
       <c r="B81" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-29</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group F</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6232,21 +6432,21 @@
         <v>1994</v>
       </c>
       <c r="B82" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-29</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group F</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6306,21 +6506,21 @@
         <v>1994</v>
       </c>
       <c r="B83" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-30</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>23:30</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group D</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6380,21 +6580,21 @@
         <v>1994</v>
       </c>
       <c r="B84" t="n">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-30</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>23:30</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group D</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6454,21 +6654,21 @@
         <v>1994</v>
       </c>
       <c r="B85" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>1994-06-26</t>
+          <t>1994-06-30</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>23:30</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Group A</t>
+          <t>Group D</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">

</xml_diff>